<commit_message>
Pila de Producto v1.1
</commit_message>
<xml_diff>
--- a/Desarrollo/BiblioTech/documentacion/Product Backlog.xlsx
+++ b/Desarrollo/BiblioTech/documentacion/Product Backlog.xlsx
@@ -804,6 +804,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -827,18 +839,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1463,8 +1463,8 @@
   </sheetPr>
   <dimension ref="B1:M70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1516,10 +1516,10 @@
       <c r="B3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
@@ -1552,18 +1552,18 @@
       <c r="B5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="47" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="44" t="s">
@@ -1595,7 +1595,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="57" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="42" t="s">
@@ -1622,7 +1622,7 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="54"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="43" t="s">
         <v>38</v>
       </c>
@@ -1647,7 +1647,7 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="47" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="43" t="s">
@@ -1672,7 +1672,7 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="56"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="43" t="s">
         <v>66</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="56"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="43" t="s">
         <v>67</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="57"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="43" t="s">
         <v>68</v>
       </c>
@@ -1747,7 +1747,7 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="47" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="42" t="s">
@@ -1772,7 +1772,7 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="56"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="42" t="s">
         <v>69</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="57"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="42" t="s">
         <v>70</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="42" t="s">
@@ -1849,7 +1849,7 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="56"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="42" t="s">
         <v>22</v>
       </c>
@@ -1874,7 +1874,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="57"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="42" t="s">
         <v>23</v>
       </c>
@@ -1899,7 +1899,7 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="47" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="42" t="s">
@@ -1924,7 +1924,7 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="56"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="42" t="s">
         <v>77</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="57"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="42" t="s">
         <v>78</v>
       </c>
@@ -1974,7 +1974,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="49" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="42" t="s">
@@ -1994,12 +1994,12 @@
         <v>3</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="58"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="42" t="s">
         <v>79</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="58"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="42" t="s">
         <v>80</v>
       </c>
@@ -2049,7 +2049,7 @@
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="58"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="42" t="s">
         <v>81</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="58"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="42" t="s">
         <v>82</v>
       </c>
@@ -2099,7 +2099,7 @@
       <c r="J26" s="9"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="47" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="42" t="s">
@@ -2124,7 +2124,7 @@
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="56"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="42" t="s">
         <v>83</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="56"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="42" t="s">
         <v>84</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="57"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="42" t="s">
         <v>85</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="42" t="s">
@@ -2224,7 +2224,7 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="56"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="42" t="s">
         <v>86</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="57"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="42" t="s">
         <v>87</v>
       </c>
@@ -2274,7 +2274,7 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="47" t="s">
         <v>64</v>
       </c>
       <c r="C34" s="42" t="s">
@@ -2299,7 +2299,7 @@
       <c r="J34" s="9"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="57"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="42" t="s">
         <v>88</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="47" t="s">
         <v>72</v>
       </c>
       <c r="C36" s="42" t="s">
@@ -2349,7 +2349,7 @@
       <c r="J36" s="9"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="57"/>
+      <c r="B37" s="48"/>
       <c r="C37" s="42" t="s">
         <v>89</v>
       </c>
@@ -2462,6 +2462,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B12"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="B22:B26"/>
@@ -2470,11 +2475,6 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B31:B33"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="J59:J60">
@@ -2932,6 +2932,25 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5124E24CAF14D46B2DD609ACFD84C07" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9971b3b784abbe199b171e233c6d3889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a36e787f936117f0a8f63b0cc0186e7" ns2:_="">
     <xsd:import namespace="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
@@ -3076,25 +3095,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09A1246-53BD-4D90-8F0D-F04270C7DF7F}">
   <ds:schemaRefs>
@@ -3104,6 +3104,38 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617ABD26-2811-4761-B5CB-14D5621085A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3119,36 +3151,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>